<commit_message>
standardized headers to camel case
</commit_message>
<xml_diff>
--- a/misc/epiparms.xlsx
+++ b/misc/epiparms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Software\spatialEpisim\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA45813-EAB2-4F88-B07E-5DBDEC84319D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7418E5-818D-4F4A-B867-1C04857637F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,9 +36,6 @@
     <t>ISONumeric</t>
   </si>
   <si>
-    <t>Model</t>
-  </si>
-  <si>
     <t>alpha</t>
   </si>
   <si>
@@ -54,25 +51,7 @@
     <t>delta</t>
   </si>
   <si>
-    <t>Lambda</t>
-  </si>
-  <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>End Date</t>
-  </si>
-  <si>
     <t>numIterations</t>
-  </si>
-  <si>
-    <t>Data Source</t>
-  </si>
-  <si>
-    <t>Disease</t>
-  </si>
-  <si>
-    <t>Scenario</t>
   </si>
   <si>
     <t>CZE</t>
@@ -100,6 +79,27 @@
   </si>
   <si>
     <t>Vaccinations</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>startDate</t>
+  </si>
+  <si>
+    <t>endDate</t>
+  </si>
+  <si>
+    <t>dataSource</t>
+  </si>
+  <si>
+    <t>disease</t>
+  </si>
+  <si>
+    <t>scenario</t>
+  </si>
+  <si>
+    <t>model</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,7 @@
   <dimension ref="A1:Y992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -516,43 +516,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>10</v>
-      </c>
       <c r="L1" s="6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -568,10 +568,10 @@
     </row>
     <row r="2" spans="1:25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C2" s="9">
         <v>0</v>
@@ -601,13 +601,13 @@
         <v>120</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
@@ -623,10 +623,10 @@
     </row>
     <row r="3" spans="1:25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C3" s="9">
         <v>0</v>
@@ -656,13 +656,13 @@
         <v>120</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
@@ -678,10 +678,10 @@
     </row>
     <row r="4" spans="1:25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C4" s="10">
         <v>1.5E-3</v>
@@ -711,13 +711,13 @@
         <v>120</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
@@ -733,10 +733,10 @@
     </row>
     <row r="5" spans="1:25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C5" s="10">
         <v>1E-4</v>
@@ -766,13 +766,13 @@
         <v>120</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>

</xml_diff>

<commit_message>
changed parameter defaults for NGA restrictions
</commit_message>
<xml_diff>
--- a/misc/epiparms.xlsx
+++ b/misc/epiparms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok Krishnamurthy\Desktop\spatialEpisim\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F7C841-F0CC-4AFE-967E-DA949B52AEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BA69C7-645D-4A9C-AF18-2D480A641434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -502,7 +502,9 @@
   </sheetPr>
   <dimension ref="A1:Y992"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -642,7 +644,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="10">
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="E3" s="9">
         <v>8.0000000000000002E-3</v>

</xml_diff>

<commit_message>
changed parameter defaults for CZE
</commit_message>
<xml_diff>
--- a/misc/epiparms.xlsx
+++ b/misc/epiparms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok Krishnamurthy\Desktop\spatialEpisim\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BA69C7-645D-4A9C-AF18-2D480A641434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4238A4-CED7-41C3-BB3C-EF248019A8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -229,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -280,6 +280,21 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -503,7 +518,7 @@
   <dimension ref="A1:Y992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -585,10 +600,10 @@
       <c r="B2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="18">
         <v>0</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="21">
         <v>0.04</v>
       </c>
       <c r="E2" s="14">
@@ -597,7 +612,7 @@
       <c r="F2" s="14">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="18">
         <v>1.5E-3</v>
       </c>
       <c r="H2" s="15">
@@ -640,10 +655,10 @@
       <c r="B3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="19">
         <v>0</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="22">
         <v>1E-3</v>
       </c>
       <c r="E3" s="9">
@@ -652,7 +667,7 @@
       <c r="F3" s="9">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="20">
         <v>1E-3</v>
       </c>
       <c r="H3" s="10">
@@ -695,11 +710,11 @@
       <c r="B4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="20">
         <v>1.5E-3</v>
       </c>
-      <c r="D4" s="10">
-        <v>2.5000000000000001E-2</v>
+      <c r="D4" s="22">
+        <v>0.03</v>
       </c>
       <c r="E4" s="9">
         <v>8.0000000000000002E-3</v>
@@ -707,7 +722,7 @@
       <c r="F4" s="9">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="19">
         <v>1.5E-3</v>
       </c>
       <c r="H4" s="10">
@@ -750,10 +765,10 @@
       <c r="B5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="20">
         <v>1E-4</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="22">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="E5" s="9">
@@ -762,7 +777,7 @@
       <c r="F5" s="9">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="20">
         <v>1E-3</v>
       </c>
       <c r="H5" s="10">

</xml_diff>

<commit_message>
changed parameter defaults for beta and delta
</commit_message>
<xml_diff>
--- a/misc/epiparms.xlsx
+++ b/misc/epiparms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok Krishnamurthy\Desktop\spatialEpisim\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4238A4-CED7-41C3-BB3C-EF248019A8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400ED2D0-D781-4830-A8A8-970617E9EF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,9 +106,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -229,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -291,10 +292,19 @@
     <xf numFmtId="165" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -518,18 +528,17 @@
   <dimension ref="A1:Y992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
@@ -603,17 +612,17 @@
       <c r="C2" s="18">
         <v>0</v>
       </c>
-      <c r="D2" s="21">
-        <v>0.04</v>
+      <c r="D2" s="25">
+        <v>0.08</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="21">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="F2" s="14">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="G2" s="18">
-        <v>1.5E-3</v>
+      <c r="G2" s="24">
+        <v>2E-3</v>
       </c>
       <c r="H2" s="15">
         <v>15</v>
@@ -658,16 +667,16 @@
       <c r="C3" s="19">
         <v>0</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="20">
         <v>1E-3</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="23">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="F3" s="9">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="22">
         <v>1E-3</v>
       </c>
       <c r="H3" s="10">
@@ -713,17 +722,17 @@
       <c r="C4" s="20">
         <v>1.5E-3</v>
       </c>
-      <c r="D4" s="22">
-        <v>0.03</v>
+      <c r="D4" s="20">
+        <v>0.05</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="23">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="F4" s="9">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="G4" s="19">
-        <v>1.5E-3</v>
+      <c r="G4" s="22">
+        <v>2E-3</v>
       </c>
       <c r="H4" s="10">
         <v>15</v>
@@ -768,16 +777,16 @@
       <c r="C5" s="20">
         <v>1E-4</v>
       </c>
-      <c r="D5" s="22">
-        <v>1.0000000000000001E-5</v>
+      <c r="D5" s="20">
+        <v>1E-4</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="23">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="F5" s="9">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="22">
         <v>1E-3</v>
       </c>
       <c r="H5" s="10">

</xml_diff>

<commit_message>
changed parameter defaults for CZE and NGA
</commit_message>
<xml_diff>
--- a/misc/epiparms.xlsx
+++ b/misc/epiparms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok Krishnamurthy\Desktop\spatialEpisim\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCDCDD7-904B-4A6C-A26A-DE9271A1AB0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076737B8-45B0-4CBD-90CC-367500A5EC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -613,7 +613,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="25">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="E2" s="21">
         <v>8.0000000000000002E-3</v>

</xml_diff>

<commit_message>
290623b Update: Updates parameter values for Uganda and DR Congo
</commit_message>
<xml_diff>
--- a/misc/epiparms.xlsx
+++ b/misc/epiparms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twhit957\Desktop\spatialEpisim\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E302A2-C2DA-4DE6-BA03-A1C458437D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62DD583-3F93-4F24-A47D-7224F437487E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -622,7 +622,7 @@
   <dimension ref="A1:Y996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -721,7 +721,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="H2" s="15">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I2" s="16">
         <v>43313</v>
@@ -886,7 +886,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="H5" s="15">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I5" s="16">
         <v>44854</v>
@@ -926,7 +926,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="23">
-        <v>0.21</v>
+        <v>1E-4</v>
       </c>
       <c r="D6" s="15">
         <v>5.4999999999999997E-3</v>
@@ -941,7 +941,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="H6" s="15">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I6" s="16">
         <v>43313</v>
@@ -1091,7 +1091,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="23">
-        <v>0.21</v>
+        <v>1E-4</v>
       </c>
       <c r="D9" s="15">
         <v>5.4999999999999997E-3</v>
@@ -1106,7 +1106,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="H9" s="15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I9" s="16">
         <v>44854</v>

</xml_diff>

<commit_message>
081623 Update: Improved generation of measuerment error covariance matrix
</commit_message>
<xml_diff>
--- a/misc/epiparms.xlsx
+++ b/misc/epiparms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twhit957\Desktop\spatialEpisim\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62DD583-3F93-4F24-A47D-7224F437487E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC544D91-6350-4261-BDB6-FA9E262602BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,10 +118,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -311,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -399,6 +400,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -622,18 +629,17 @@
   <dimension ref="A1:Y996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
@@ -705,7 +711,7 @@
       <c r="B2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="23">
+      <c r="C2" s="31">
         <v>0</v>
       </c>
       <c r="D2" s="15">
@@ -760,7 +766,7 @@
       <c r="B3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="31">
         <v>0</v>
       </c>
       <c r="D3" s="23">
@@ -815,7 +821,7 @@
       <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="32">
         <v>0</v>
       </c>
       <c r="D4" s="18">
@@ -870,7 +876,7 @@
       <c r="B5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="31">
         <v>0</v>
       </c>
       <c r="D5" s="15">
@@ -925,23 +931,23 @@
       <c r="B6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="23">
-        <v>1E-4</v>
+      <c r="C6" s="31">
+        <v>3.4999999999999997E-5</v>
       </c>
       <c r="D6" s="15">
-        <v>5.4999999999999997E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="E6" s="14">
-        <v>5.4999999999999997E-3</v>
+        <v>0.14285709999999999</v>
       </c>
       <c r="F6" s="14">
-        <v>0.01</v>
+        <v>2.7777779999999998E-2</v>
       </c>
       <c r="G6" s="15">
-        <v>2.1000000000000001E-2</v>
+        <v>5.5555559999999997E-2</v>
       </c>
       <c r="H6" s="15">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I6" s="16">
         <v>43313</v>
@@ -950,7 +956,7 @@
         <v>43753</v>
       </c>
       <c r="K6" s="14">
-        <v>440</v>
+        <v>689</v>
       </c>
       <c r="L6" s="14" t="s">
         <v>25</v>
@@ -980,7 +986,7 @@
       <c r="B7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="32">
         <v>1.5E-3</v>
       </c>
       <c r="D7" s="18">
@@ -1035,7 +1041,7 @@
       <c r="B8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="32">
         <v>1E-4</v>
       </c>
       <c r="D8" s="18">
@@ -1090,7 +1096,7 @@
       <c r="B9" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="31">
         <v>1E-4</v>
       </c>
       <c r="D9" s="15">

</xml_diff>

<commit_message>
082123: Changes made by TBW
</commit_message>
<xml_diff>
--- a/misc/epiparms.xlsx
+++ b/misc/epiparms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twhit957\Desktop\spatialEpisim\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC544D91-6350-4261-BDB6-FA9E262602BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AE2EF3-8E5D-4624-AC0B-1F98DA4F6222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -628,9 +628,7 @@
   </sheetPr>
   <dimension ref="A1:Y996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -901,7 +899,7 @@
         <v>44936</v>
       </c>
       <c r="K5" s="28">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="L5" s="28" t="s">
         <v>25</v>
@@ -1097,22 +1095,22 @@
         <v>14</v>
       </c>
       <c r="C9" s="31">
-        <v>1E-4</v>
+        <v>3.4999999999999997E-5</v>
       </c>
       <c r="D9" s="15">
-        <v>5.4999999999999997E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="E9" s="14">
-        <v>5.4999999999999997E-3</v>
+        <v>0.14285700000000001</v>
       </c>
       <c r="F9" s="14">
-        <v>0.01</v>
+        <v>2.7777799999999998E-2</v>
       </c>
       <c r="G9" s="15">
-        <v>2.1000000000000001E-2</v>
+        <v>5.5555599999999997E-2</v>
       </c>
       <c r="H9" s="15">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="I9" s="16">
         <v>44854</v>
@@ -1121,7 +1119,7 @@
         <v>44936</v>
       </c>
       <c r="K9" s="28">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="L9" s="28" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
COD SVEIRD parameters changed Apr 9
</commit_message>
<xml_diff>
--- a/misc/epiparms.xlsx
+++ b/misc/epiparms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashok\Desktop\spatialEpisim2022\spatialEpisim\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E061FA9C-BBB1-4577-A186-545F1D320F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C419A9-5779-49FD-9C5B-D129811FA33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -629,7 +629,7 @@
   <dimension ref="A1:Y996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -935,16 +935,16 @@
         <v>3.4999999999999997E-5</v>
       </c>
       <c r="D6" s="15">
-        <v>5.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="E6" s="14">
+        <v>1.5E-3</v>
+      </c>
+      <c r="F6" s="14">
         <v>0.01</v>
       </c>
-      <c r="F6" s="14">
-        <v>0.03</v>
-      </c>
       <c r="G6" s="15">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="H6" s="15">
         <v>15</v>
@@ -956,7 +956,7 @@
         <v>43753</v>
       </c>
       <c r="K6" s="14">
-        <v>440</v>
+        <v>689</v>
       </c>
       <c r="L6" s="14" t="s">
         <v>25</v>

</xml_diff>